<commit_message>
succesfully reading all nvessels tables
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb44/raw/Table30.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb44/raw/Table30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb44/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5024900-67DC-3B48-9C12-652A5E770FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2934BD41-E5BE-A849-9272-4975B566F49B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Regions of home ports</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Total number of boats in each region</t>
+  </si>
+  <si>
+    <t>Monterey</t>
+  </si>
+  <si>
+    <t>Santa Barbara</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
   </si>
 </sst>
 </file>
@@ -83,7 +92,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -159,17 +168,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -491,10 +500,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23"/>
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -664,8 +673,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" s="10">
         <v>67</v>
       </c>
@@ -689,8 +700,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B8" s="10">
         <v>35</v>
       </c>
@@ -714,8 +727,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="B9" s="10">
         <v>124</v>
       </c>
@@ -766,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -793,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
         <v>13</v>
       </c>

</xml_diff>